<commit_message>
ADD threads for CRUD BBDD
</commit_message>
<xml_diff>
--- a/datos_exportados_Clientes.xlsx
+++ b/datos_exportados_Clientes.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="155">
   <si>
     <t>DNI_Cliente</t>
   </si>
@@ -53,6 +53,21 @@
     <t>abdel@gmail.com</t>
   </si>
   <si>
+    <t>002255889P</t>
+  </si>
+  <si>
+    <t>Sara</t>
+  </si>
+  <si>
+    <t>Rodriguez 3</t>
+  </si>
+  <si>
+    <t>C/ Canciones malas</t>
+  </si>
+  <si>
+    <t>sara.33@gmail.com</t>
+  </si>
+  <si>
     <t>021245789C</t>
   </si>
   <si>
@@ -129,9 +144,6 @@
   </si>
   <si>
     <t>024579642C</t>
-  </si>
-  <si>
-    <t>Sara</t>
   </si>
   <si>
     <t>RC</t>
@@ -509,7 +521,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -572,7 +584,7 @@
         <v>15</v>
       </c>
       <c r="D3" t="n">
-        <v>6.58775112E8</v>
+        <v>6987412.0</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
@@ -595,7 +607,7 @@
         <v>20</v>
       </c>
       <c r="D4" t="n">
-        <v>9.1919191E7</v>
+        <v>6.58775112E8</v>
       </c>
       <c r="E4" t="s">
         <v>21</v>
@@ -618,62 +630,62 @@
         <v>25</v>
       </c>
       <c r="D5" t="n">
-        <v>6.58741236E8</v>
+        <v>9.1919191E7</v>
       </c>
       <c r="E5" t="s">
         <v>26</v>
       </c>
       <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
         <v>27</v>
-      </c>
-      <c r="G5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
         <v>29</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>30</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="n">
+        <v>6.58741236E8</v>
+      </c>
+      <c r="E6" t="s">
         <v>31</v>
       </c>
-      <c r="D6" t="n">
-        <v>6.58745672E8</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>32</v>
       </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D7" t="n">
-        <v>6.9964564E7</v>
+        <v>6.58745672E8</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
@@ -687,39 +699,39 @@
         <v>40</v>
       </c>
       <c r="D8" t="n">
-        <v>2.147483647E9</v>
+        <v>6.9964564E7</v>
       </c>
       <c r="E8" t="s">
         <v>41</v>
       </c>
       <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" t="s">
         <v>42</v>
-      </c>
-      <c r="G8" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
         <v>44</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="n">
+        <v>2.147483647E9</v>
+      </c>
+      <c r="E9" t="s">
         <v>45</v>
       </c>
-      <c r="C9" t="s">
+      <c r="F9" t="s">
         <v>46</v>
       </c>
-      <c r="D9" t="n">
-        <v>8.72458833E8</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>47</v>
-      </c>
-      <c r="F9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="10">
@@ -733,7 +745,7 @@
         <v>50</v>
       </c>
       <c r="D10" t="n">
-        <v>6.9958978E7</v>
+        <v>8.72458833E8</v>
       </c>
       <c r="E10" t="s">
         <v>51</v>
@@ -742,53 +754,53 @@
         <v>11</v>
       </c>
       <c r="G10" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
         <v>53</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>54</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="n">
+        <v>6.9958978E7</v>
+      </c>
+      <c r="E11" t="s">
         <v>55</v>
       </c>
-      <c r="D11" t="n">
-        <v>2.25947126E8</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s">
         <v>56</v>
-      </c>
-      <c r="F11" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" t="s">
         <v>59</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="n">
+        <v>2.25947126E8</v>
+      </c>
+      <c r="E12" t="s">
         <v>60</v>
       </c>
-      <c r="C12" t="s">
+      <c r="F12" t="s">
         <v>61</v>
       </c>
-      <c r="D12" t="n">
-        <v>6.99874126E8</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="G12" t="s">
         <v>62</v>
-      </c>
-      <c r="F12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="13">
@@ -802,7 +814,7 @@
         <v>65</v>
       </c>
       <c r="D13" t="n">
-        <v>6.58754687E8</v>
+        <v>6.99874126E8</v>
       </c>
       <c r="E13" t="s">
         <v>66</v>
@@ -825,7 +837,7 @@
         <v>69</v>
       </c>
       <c r="D14" t="n">
-        <v>9.87567752E8</v>
+        <v>6.58754687E8</v>
       </c>
       <c r="E14" t="s">
         <v>70</v>
@@ -834,99 +846,99 @@
         <v>11</v>
       </c>
       <c r="G14" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
         <v>72</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>73</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="n">
+        <v>9.87567752E8</v>
+      </c>
+      <c r="E15" t="s">
         <v>74</v>
       </c>
-      <c r="D15" t="n">
-        <v>1.1111111E7</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" t="s">
         <v>75</v>
-      </c>
-      <c r="F15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" t="s">
         <v>77</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>78</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="n">
+        <v>1.1111111E7</v>
+      </c>
+      <c r="E16" t="s">
         <v>79</v>
       </c>
-      <c r="D16" t="n">
-        <v>9.5123578E7</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" t="s">
         <v>80</v>
-      </c>
-      <c r="F16" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" t="s">
         <v>82</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>83</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="n">
+        <v>9.5123578E7</v>
+      </c>
+      <c r="E17" t="s">
         <v>84</v>
       </c>
-      <c r="D17" t="n">
-        <v>2.147483647E9</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" t="s">
         <v>85</v>
-      </c>
-      <c r="F17" t="s">
-        <v>86</v>
-      </c>
-      <c r="G17" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" t="s">
         <v>88</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" t="n">
+        <v>2.147483647E9</v>
+      </c>
+      <c r="E18" t="s">
         <v>89</v>
       </c>
-      <c r="C18" t="s">
+      <c r="F18" t="s">
         <v>90</v>
       </c>
-      <c r="D18" t="n">
-        <v>6.99857412E8</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="G18" t="s">
         <v>91</v>
-      </c>
-      <c r="F18" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="19">
@@ -934,203 +946,203 @@
         <v>92</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D19" t="n">
-        <v>9.87456321E8</v>
+        <v>6.99857412E8</v>
       </c>
       <c r="E19" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F19" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="G19" t="s">
-        <v>94</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B20" t="s">
-        <v>96</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" t="n">
+        <v>9.87456321E8</v>
+      </c>
+      <c r="E20" t="s">
         <v>97</v>
       </c>
-      <c r="D20" t="n">
-        <v>6.99029507E8</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" t="s">
         <v>98</v>
-      </c>
-      <c r="F20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G20" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" t="s">
         <v>100</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>101</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="n">
+        <v>6.99029507E8</v>
+      </c>
+      <c r="E21" t="s">
         <v>102</v>
       </c>
-      <c r="D21" t="n">
-        <v>6.90019403E8</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" t="s">
         <v>103</v>
-      </c>
-      <c r="F21" t="s">
-        <v>104</v>
-      </c>
-      <c r="G21" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" t="s">
         <v>106</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D22" t="n">
+        <v>6.90019403E8</v>
+      </c>
+      <c r="E22" t="s">
         <v>107</v>
       </c>
-      <c r="C22" t="s">
+      <c r="F22" t="s">
         <v>108</v>
       </c>
-      <c r="D22" t="n">
-        <v>6.66665568E8</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="G22" t="s">
         <v>109</v>
-      </c>
-      <c r="F22" t="s">
-        <v>27</v>
-      </c>
-      <c r="G22" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" t="s">
         <v>111</v>
-      </c>
-      <c r="B23" t="s">
-        <v>30</v>
       </c>
       <c r="C23" t="s">
         <v>112</v>
       </c>
       <c r="D23" t="n">
-        <v>6.5842597E7</v>
+        <v>6.66665568E8</v>
       </c>
       <c r="E23" t="s">
         <v>113</v>
       </c>
       <c r="F23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G23" t="s">
         <v>114</v>
-      </c>
-      <c r="G23" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" t="s">
         <v>116</v>
       </c>
-      <c r="B24" t="s">
-        <v>96</v>
-      </c>
-      <c r="C24" t="s">
-        <v>97</v>
-      </c>
       <c r="D24" t="n">
-        <v>6.99029507E8</v>
+        <v>6.5842597E7</v>
       </c>
       <c r="E24" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="F24" t="s">
-        <v>27</v>
+        <v>118</v>
       </c>
       <c r="G24" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B25" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="C25" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="D25" t="n">
-        <v>6.4547375E7</v>
+        <v>6.99029507E8</v>
       </c>
       <c r="E25" t="s">
+        <v>102</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" t="s">
         <v>121</v>
-      </c>
-      <c r="F25" t="s">
-        <v>27</v>
-      </c>
-      <c r="G25" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" t="s">
         <v>123</v>
       </c>
-      <c r="B26" t="s">
-        <v>24</v>
-      </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>124</v>
       </c>
       <c r="D26" t="n">
-        <v>6.5822387E7</v>
+        <v>6.4547375E7</v>
       </c>
       <c r="E26" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F26" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G26" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B27" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>127</v>
+        <v>8</v>
       </c>
       <c r="D27" t="n">
-        <v>6.58745236E8</v>
+        <v>6.5822387E7</v>
       </c>
       <c r="E27" t="s">
         <v>128</v>
       </c>
       <c r="F27" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G27" t="s">
         <v>129</v>
@@ -1141,22 +1153,22 @@
         <v>130</v>
       </c>
       <c r="B28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" t="s">
         <v>131</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="n">
+        <v>6.58745236E8</v>
+      </c>
+      <c r="E28" t="s">
         <v>132</v>
       </c>
-      <c r="D28" t="n">
-        <v>6.58996478E8</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28" t="s">
         <v>133</v>
-      </c>
-      <c r="F28" t="s">
-        <v>11</v>
-      </c>
-      <c r="G28" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="29">
@@ -1170,62 +1182,85 @@
         <v>136</v>
       </c>
       <c r="D29" t="n">
-        <v>6.58746677E8</v>
+        <v>6.58996478E8</v>
       </c>
       <c r="E29" t="s">
         <v>137</v>
       </c>
       <c r="F29" t="s">
-        <v>138</v>
+        <v>11</v>
       </c>
       <c r="G29" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
+        <v>138</v>
+      </c>
+      <c r="B30" t="s">
+        <v>139</v>
+      </c>
+      <c r="C30" t="s">
         <v>140</v>
       </c>
-      <c r="B30" t="s">
+      <c r="D30" t="n">
+        <v>6.58746677E8</v>
+      </c>
+      <c r="E30" t="s">
         <v>141</v>
       </c>
-      <c r="C30" t="s">
+      <c r="F30" t="s">
         <v>142</v>
       </c>
-      <c r="D30" t="n">
-        <v>1.23456789E8</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="G30" t="s">
         <v>143</v>
-      </c>
-      <c r="F30" t="s">
-        <v>144</v>
-      </c>
-      <c r="G30" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B31" t="s">
+        <v>145</v>
+      </c>
+      <c r="C31" t="s">
         <v>146</v>
       </c>
-      <c r="B31" t="s">
+      <c r="D31" t="n">
+        <v>1.23456789E8</v>
+      </c>
+      <c r="E31" t="s">
         <v>147</v>
       </c>
-      <c r="C31" t="s">
+      <c r="F31" t="s">
         <v>148</v>
       </c>
-      <c r="D31" t="n">
+      <c r="G31" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>150</v>
+      </c>
+      <c r="B32" t="s">
+        <v>151</v>
+      </c>
+      <c r="C32" t="s">
+        <v>152</v>
+      </c>
+      <c r="D32" t="n">
         <v>4.5613345E7</v>
       </c>
-      <c r="E31" t="s">
-        <v>149</v>
-      </c>
-      <c r="F31" t="s">
-        <v>27</v>
-      </c>
-      <c r="G31" t="s">
-        <v>150</v>
+      <c r="E32" t="s">
+        <v>153</v>
+      </c>
+      <c r="F32" t="s">
+        <v>32</v>
+      </c>
+      <c r="G32" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>